<commit_message>
updated charts with dynamic hours in the text boxes
</commit_message>
<xml_diff>
--- a/static/work-tracker.xlsx
+++ b/static/work-tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UQAM\Personnel\Sérieux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F99272F-0526-4456-A936-21C65D1031C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93C02B-6E03-4AA8-87E2-B4D8B526B364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" xr2:uid="{4E48D71A-11A8-48A3-A37D-9541A381940A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" activeTab="3" xr2:uid="{4E48D71A-11A8-48A3-A37D-9541A381940A}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>Monday</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>At the end of your work week, add your total daily hours worked for each day of that week in the appropriate cells (Monday to Sunday).</t>
+  </si>
+  <si>
+    <t>Objective: 40 hrs/week (5 day x 8 hrs)</t>
   </si>
 </sst>
 </file>
@@ -5120,7 +5123,7 @@
       <cdr:x>0.63767</cdr:x>
       <cdr:y>0.80921</cdr:y>
     </cdr:to>
-    <cdr:sp macro="" textlink="">
+    <cdr:sp macro="" textlink="'Fall 2019'!$W$43">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -5153,31 +5156,17 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1"/>
-            <a:t>Average:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t> 38.75 hrs/week</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>Objective: 40 hrs/week (5</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1">
-              <a:effectLst/>
+          <a:fld id="{5C4B9791-3BAC-4824-99C4-05005AA4E0DE}" type="TxLink">
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t> day x 8 hrs</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>)</a:t>
-          </a:r>
+            <a:t>Average: 38.75 hrs/week
+Objective: 40 hrs/week (5 day x 8 hrs)</a:t>
+          </a:fld>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
       </cdr:txBody>
@@ -5719,7 +5708,7 @@
       <cdr:x>0.56913</cdr:x>
       <cdr:y>0.73377</cdr:y>
     </cdr:to>
-    <cdr:sp macro="" textlink="">
+    <cdr:sp macro="" textlink="'Winter 2020'!$W$43">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -5752,31 +5741,17 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1"/>
-            <a:t>Average:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t> 28.06 hrs/week</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>Objective: 40 hrs/week (5</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1">
-              <a:effectLst/>
+          <a:fld id="{F31EDC80-FAF2-4CF9-BA31-0B6B1413961A}" type="TxLink">
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t> day x 8 hrs</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>)</a:t>
-          </a:r>
+            <a:t>Average: 28.06 hrs/week
+Objective: 40 hrs/week (5 day x 8 hrs)</a:t>
+          </a:fld>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
       </cdr:txBody>
@@ -6632,7 +6607,7 @@
       <cdr:x>0.5193</cdr:x>
       <cdr:y>0.72272</cdr:y>
     </cdr:to>
-    <cdr:sp macro="" textlink="">
+    <cdr:sp macro="" textlink="'Summer 2020'!$W$43">
       <cdr:nvSpPr>
         <cdr:cNvPr id="2" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -6665,31 +6640,17 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1"/>
-            <a:t>Average:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t> 39.78 hrs/week</a:t>
-          </a:r>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>Objective: 40 hrs/week (5</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1">
-              <a:effectLst/>
+          <a:fld id="{4C15B898-325F-4C4E-A3A0-6A7982899CDA}" type="TxLink">
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t> day x 8 hrs</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" b="1" baseline="0"/>
-            <a:t>)</a:t>
-          </a:r>
+            <a:t>Average: 39.78 hrs/week
+Objective: 40 hrs/week (5 day x 8 hrs)</a:t>
+          </a:fld>
           <a:endParaRPr lang="en-CA" sz="1100" b="1"/>
         </a:p>
       </cdr:txBody>
@@ -7162,7 +7123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B6FE27-0780-44AF-82FB-9A1F916D752A}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -7292,8 +7253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF153EC7-E9DA-4693-BC09-732742EBE1D6}">
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8347,14 +8308,32 @@
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="L30" s="1"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W38" t="str">
+        <f>_xlfn.CONCAT("Average: ", ROUND(INDEX(K2:K19,MATCH(1E+100,I2:I19,1)), 2), " hrs/week")</f>
+        <v>Average: 38.75 hrs/week</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="W43" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(CHAR(10), FALSE, W38:W39)</f>
+        <v>Average: 38.75 hrs/week
+Objective: 40 hrs/week (5 day x 8 hrs)</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -8457,10 +8436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F338CE8E-79C9-4031-AEC0-0D5175012249}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9506,6 +9485,24 @@
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="L30" s="1"/>
     </row>
+    <row r="38" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W38" t="str">
+        <f>_xlfn.CONCAT("Average: ", ROUND(INDEX(K2:K19,MATCH(1E+100,I2:I19,1)), 2), " hrs/week")</f>
+        <v>Average: 28.06 hrs/week</v>
+      </c>
+    </row>
+    <row r="39" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="23:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="W43" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(CHAR(10), FALSE, W38:W39)</f>
+        <v>Average: 28.06 hrs/week
+Objective: 40 hrs/week (5 day x 8 hrs)</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9515,10 +9512,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735939E8-15A8-49BB-845D-CC0815CA17CA}">
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10394,6 +10391,24 @@
         <v>35</v>
       </c>
     </row>
+    <row r="38" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W38" t="str">
+        <f>_xlfn.CONCAT("Average: ", ROUND(INDEX(K2:K19,MATCH(1E+100,I2:I19,1)), 2), " hrs/week")</f>
+        <v>Average: 39.78 hrs/week</v>
+      </c>
+    </row>
+    <row r="39" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="23:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="W43" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(CHAR(10), FALSE, W38:W39)</f>
+        <v>Average: 39.78 hrs/week
+Objective: 40 hrs/week (5 day x 8 hrs)</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated instructions of work-trackers
</commit_message>
<xml_diff>
--- a/static/work-tracker.xlsx
+++ b/static/work-tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UQAM\Personnel\Sérieux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UQAM\GitHub\starter-academic\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A93C02B-6E03-4AA8-87E2-B4D8B526B364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D45684-EAFD-4BA6-8F14-137A48799502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" activeTab="3" xr2:uid="{4E48D71A-11A8-48A3-A37D-9541A381940A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" xr2:uid="{4E48D71A-11A8-48A3-A37D-9541A381940A}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="13" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>After getting the idea, you can erase the existing example data (the sample hours worked, not the rest) before you start tracking your own hours.</t>
   </si>
   <si>
-    <t>You can edit the summary box (white background) with your current number of hours worked and objective.</t>
-  </si>
-  <si>
     <t>Blog post:</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Objective: 40 hrs/week (5 day x 8 hrs)</t>
+  </si>
+  <si>
+    <t>The summary box (white background) will update automatically with your current number of hours worked and objective.</t>
   </si>
 </sst>
 </file>
@@ -5164,6 +5164,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>Average: 38.75 hrs/week
 Objective: 40 hrs/week (5 day x 8 hrs)</a:t>
           </a:fld>
@@ -5749,6 +5750,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>Average: 28.06 hrs/week
 Objective: 40 hrs/week (5 day x 8 hrs)</a:t>
           </a:fld>
@@ -6648,6 +6650,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr algn="ctr"/>
             <a:t>Average: 39.78 hrs/week
 Objective: 40 hrs/week (5 day x 8 hrs)</a:t>
           </a:fld>
@@ -7123,8 +7126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B6FE27-0780-44AF-82FB-9A1F916D752A}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7158,7 +7161,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7195,7 +7198,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7214,7 +7217,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -7253,7 +7256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF153EC7-E9DA-4693-BC09-732742EBE1D6}">
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
@@ -8316,7 +8319,7 @@
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="W39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:23" ht="30" x14ac:dyDescent="0.25">
@@ -8438,7 +8441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F338CE8E-79C9-4031-AEC0-0D5175012249}">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -9493,7 +9496,7 @@
     </row>
     <row r="39" spans="23:23" x14ac:dyDescent="0.25">
       <c r="W39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="23:23" ht="30" x14ac:dyDescent="0.25">
@@ -9514,7 +9517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735939E8-15A8-49BB-845D-CC0815CA17CA}">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
@@ -10399,10 +10402,10 @@
     </row>
     <row r="39" spans="23:23" x14ac:dyDescent="0.25">
       <c r="W39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="23:23" ht="60" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="23:23" ht="30" x14ac:dyDescent="0.25">
       <c r="W43" s="2" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(10), FALSE, W38:W39)</f>
         <v>Average: 39.78 hrs/week

</xml_diff>

<commit_message>
updated work trackers a bit
</commit_message>
<xml_diff>
--- a/static/work-tracker.xlsx
+++ b/static/work-tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UQAM\GitHub\starter-academic\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UQAM\Personnel\Sérieux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D45684-EAFD-4BA6-8F14-137A48799502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB9A832-450E-4174-9004-3515A13DFC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="717" xr2:uid="{4E48D71A-11A8-48A3-A37D-9541A381940A}"/>
   </bookViews>
@@ -7256,7 +7256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF153EC7-E9DA-4693-BC09-732742EBE1D6}">
   <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
@@ -8441,7 +8441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F338CE8E-79C9-4031-AEC0-0D5175012249}">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -9517,7 +9517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735939E8-15A8-49BB-845D-CC0815CA17CA}">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>

</xml_diff>